<commit_message>
Final experiments with dropout
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabim\Documents\Master\CentraleSupelec\DeepLearning\Assignments\Assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B68232A-F2C3-4A78-B83F-55B447CBA06C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576AAAA7-663E-406D-B23D-593C47459124}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9D8F4F1-2B52-4661-A271-B09CCEFFBCEE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Training</t>
   </si>
@@ -92,12 +92,18 @@
   </si>
   <si>
     <t>Variation training vs test</t>
+  </si>
+  <si>
+    <t>Dropout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,6 +390,30 @@
     <xf numFmtId="10" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,28 +441,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -749,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17245CD8-AA79-4986-B54F-A5911C9F3098}">
-  <dimension ref="E6:J20"/>
+  <dimension ref="E6:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D15" zoomScale="149" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D18" zoomScale="149" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -768,11 +786,11 @@
     <row r="6" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="5:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E7" s="4" t="s">
@@ -792,7 +810,7 @@
       </c>
     </row>
     <row r="8" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="36" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -809,7 +827,7 @@
       </c>
     </row>
     <row r="9" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="29"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="12" t="s">
         <v>5</v>
       </c>
@@ -824,7 +842,7 @@
       </c>
     </row>
     <row r="10" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="30"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="15" t="s">
         <v>6</v>
       </c>
@@ -839,7 +857,7 @@
       </c>
     </row>
     <row r="11" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="39" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="18" t="s">
@@ -856,7 +874,7 @@
       </c>
     </row>
     <row r="12" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="32"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="21" t="s">
         <v>5</v>
       </c>
@@ -871,7 +889,7 @@
       </c>
     </row>
     <row r="13" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="33"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="15" t="s">
         <v>6</v>
       </c>
@@ -888,11 +906,11 @@
     <row r="17" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
     </row>
     <row r="18" spans="5:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E18" s="4" t="s">
@@ -910,12 +928,12 @@
       <c r="I18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="39" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -930,32 +948,122 @@
       <c r="I19" s="13">
         <v>0.9788</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="32">
         <f>(I19/100)/(G19/100)-1</f>
         <v>-1.3107481347045757E-2</v>
       </c>
     </row>
     <row r="20" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="33"/>
-      <c r="F20" s="37" t="s">
+      <c r="E20" s="41"/>
+      <c r="F20" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="29">
         <v>0.99890000000000001</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="30">
         <v>0.98109999999999997</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="29">
         <v>0.98050000000000004</v>
       </c>
-      <c r="J20" s="41">
+      <c r="J20" s="32">
         <f>(I20/100)/(G20/100)-1</f>
         <v>-1.8420262288517231E-2</v>
       </c>
     </row>
+    <row r="23" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="34"/>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="5:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="E24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.99890000000000001</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0.98070000000000002</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="J25" s="45">
+        <f>(I25/100)/(G25/100)-1</f>
+        <v>-1.7319050956051574E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="40"/>
+      <c r="F26" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="43">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="H26" s="44">
+        <v>0.97940000000000005</v>
+      </c>
+      <c r="I26" s="43">
+        <v>0.9788</v>
+      </c>
+      <c r="J26" s="45">
+        <f>(I26/100)/(G26/100)-1</f>
+        <v>-1.3107481347045757E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="41"/>
+      <c r="F27" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="29">
+        <v>0.99890000000000001</v>
+      </c>
+      <c r="H27" s="30">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="I27" s="29">
+        <v>0.98050000000000004</v>
+      </c>
+      <c r="J27" s="45">
+        <f>(I27/100)/(G27/100)-1</f>
+        <v>-1.8420262288517231E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E25:E27"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="E11:E13"/>
@@ -996,13 +1104,13 @@
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1010,16 +1118,16 @@
       <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="36">
         <v>300</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="36">
         <v>8000</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="36">
         <v>0.01</v>
       </c>
     </row>
@@ -1027,19 +1135,19 @@
       <c r="E9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
     </row>
     <row r="10" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="5:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E11" s="2"/>

</xml_diff>